<commit_message>
Ready to find next slow function
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT\Summer_school\HashTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCAE7C1-0045-4A42-9C29-06A7C2CE2136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66882FAA-2FC5-455C-A7CD-70A7BFE80D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,15 +634,15 @@
         <v>523.38613999999995</v>
       </c>
       <c r="D18">
-        <f>D6/$C$1</f>
+        <f t="shared" ref="D18:F26" si="1">D6/$C$1</f>
         <v>190.94556</v>
       </c>
       <c r="E18">
-        <f>E6/$C$1</f>
+        <f t="shared" si="1"/>
         <v>96.857039999999998</v>
       </c>
       <c r="F18">
-        <f>F6/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -655,15 +655,15 @@
         <v>531.47770000000003</v>
       </c>
       <c r="D19">
-        <f>D7/$C$1</f>
+        <f t="shared" si="1"/>
         <v>183.12508</v>
       </c>
       <c r="E19">
-        <f>E7/$C$1</f>
+        <f t="shared" si="1"/>
         <v>112.62764</v>
       </c>
       <c r="F19">
-        <f>F7/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -676,15 +676,15 @@
         <v>533.66804000000002</v>
       </c>
       <c r="D20">
-        <f>D8/$C$1</f>
+        <f t="shared" si="1"/>
         <v>194.97183999999999</v>
       </c>
       <c r="E20">
-        <f>E8/$C$1</f>
+        <f t="shared" si="1"/>
         <v>107.66592</v>
       </c>
       <c r="F20">
-        <f>F8/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -697,15 +697,15 @@
         <v>561.89</v>
       </c>
       <c r="D21">
-        <f>D9/$C$1</f>
+        <f t="shared" si="1"/>
         <v>189.34526</v>
       </c>
       <c r="E21">
-        <f>E9/$C$1</f>
+        <f t="shared" si="1"/>
         <v>106.34004</v>
       </c>
       <c r="F21">
-        <f>F9/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -718,15 +718,15 @@
         <v>532.16782000000001</v>
       </c>
       <c r="D22">
-        <f>D10/$C$1</f>
+        <f t="shared" si="1"/>
         <v>192.02724000000001</v>
       </c>
       <c r="E22">
-        <f>E10/$C$1</f>
+        <f t="shared" si="1"/>
         <v>100.40461999999999</v>
       </c>
       <c r="F22">
-        <f>F10/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -739,15 +739,15 @@
         <v>536.53926000000001</v>
       </c>
       <c r="D23">
-        <f>D11/$C$1</f>
+        <f t="shared" si="1"/>
         <v>189.97573</v>
       </c>
       <c r="E23">
-        <f>E11/$C$1</f>
+        <f t="shared" si="1"/>
         <v>108.23112</v>
       </c>
       <c r="F23">
-        <f>F11/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -760,15 +760,15 @@
         <v>551.29862000000003</v>
       </c>
       <c r="D24">
-        <f>D12/$C$1</f>
+        <f t="shared" si="1"/>
         <v>177.15544</v>
       </c>
       <c r="E24">
-        <f>E12/$C$1</f>
+        <f t="shared" si="1"/>
         <v>121.32953999999999</v>
       </c>
       <c r="F24">
-        <f>F12/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -781,15 +781,15 @@
         <v>532.84474</v>
       </c>
       <c r="D25">
-        <f>D13/$C$1</f>
+        <f t="shared" si="1"/>
         <v>183.23133999999999</v>
       </c>
       <c r="E25">
-        <f>E13/$C$1</f>
+        <f t="shared" si="1"/>
         <v>107.00539999999999</v>
       </c>
       <c r="F25">
-        <f>F13/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -802,15 +802,15 @@
         <v>532.57776000000001</v>
       </c>
       <c r="D26">
-        <f>D14/$C$1</f>
+        <f t="shared" si="1"/>
         <v>214.45310000000001</v>
       </c>
       <c r="E26">
-        <f>E14/$C$1</f>
+        <f t="shared" si="1"/>
         <v>96.682500000000005</v>
       </c>
       <c r="F26">
-        <f>F14/$C$1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -886,11 +886,11 @@
         <v>2.8178739604430634</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" ref="E32:F32" si="1">D28/E28</f>
+        <f t="shared" ref="E32:F32" si="2">D28/E28</f>
         <v>1.7980990861900057</v>
       </c>
       <c r="F32" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added hash distribution research
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT\Summer_school\HashTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25908B1F-86D0-481B-A0E2-CFAE22FDC49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDC4E98-8977-4792-BF04-46F4A9B8386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1171,6 +1171,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <f>C28/H28</f>
+        <v>5.5909795785763077</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>